<commit_message>
feat: fixed stupid team id bug
</commit_message>
<xml_diff>
--- a/id_schedule.xlsx
+++ b/id_schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Friedman 102</t>
+          <t>Friedman 108</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -461,844 +461,537 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Salomon 003</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Salomon 004</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Salomon 202</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Salomon 203</t>
+          <t>Friedman 208</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>12:00</t>
+          <t>12:10</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>down-chimpanzee-drain-surprisingly-prhi</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>dumb-commissioner-chew-loudly</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>disgraced-pairing-interest-beautifully-first</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>helpful-beginner-mend-exactly-prhi</t>
+          <t>oncoming-dossier-print-fortunately-first</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>grouchy-depression-save-properly</t>
+          <t>worsted-bending-record-playfully-first</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>worsted-nylon-tour-knottily-prhi</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>subjective-resurgence-repaired-yawningly-prhi</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>combined-saucer-destroy-sedately</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
+          <t>inoffensive-sesame-shaded-beautifully</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>12:10</t>
+          <t>12:17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>burial-mahogany-flash-fully-prhi</t>
+          <t>greener-mango-mended-yearly-first</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>charcoal-balls-introduced-honestly</t>
+          <t>productive-brunch-scolded-really-first</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>subordinate-lineage-divided-kookily-prhi</t>
+          <t>enlightened-sufferer-observe-truthfully</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>summary-inevitability-flooded-delightfully</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>deprived-outfield-wink-swiftly-prhi</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>12:20</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>realistic-elk-faced-questionably</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+          <t>12:24</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>lonely-aggression-cheer-frightfully</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>small-aardvark-precede-shrilly-first</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>comparable-allies-lightened-yesterday</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>devastating-drilling-reported-successfully-prhi</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>disconnected-brewer-escaped-upbeat</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>intimate-instructor-sparkle-sharply-prhi</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
+          <t>content-raccoon-snored-coaxingly-first</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>12:30</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
+          <t>12:31</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>detective-hierarchy-answer-nervously</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>calm-owner-chopped-upright</t>
+          <t>haunting-widget-damaged-generally-first</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>handicapped-putting-bolted-bravely</t>
+          <t>responsible-solemnity-rinse-wetly</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>incalculable-validity-signed-somewhat</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>fanciful-rationality-attempted-longingly</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>united-syrah-repaired-somewhat</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>exacting-touchdown-picked-loudly</t>
-        </is>
-      </c>
+          <t>frightened-maple-succeed-madly</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>12:40</t>
+          <t>12:38</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>insane-armadillo-clap-deceivingly-prhi</t>
+          <t>funny-reader-added-kindly</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>slamming-locality-mess up-quizzically-prhi</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>intimate-instructor-sparkle-sharply-prhi</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>neutered-pathos-drip-fast-prhi</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>electoral-terry-employ-silently-prhi</t>
+          <t>haunted-repayment-tip-vainly-first</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>utter-clothing-fixed-playfully</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>flowing-darkness-competed-terribly</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>12:50</t>
+          <t>12:45</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>interpreted-reptile-groan-anxiously-prhi</t>
+          <t>endangered-interval-practised-meaningfully-first</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>young-canary-pleased-heavily-prhi</t>
+          <t>deodorant-legislation-subtract-kiddingly-first</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>liver-laurels-asked-tediously-prhi</t>
+          <t>noticed-outset-tired-less</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>geometric-fastball-suppose-owlishly-prhi</t>
+          <t>halfbreed-hardship-relax-merrily</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>wellinformed-tansy-prepared-annually</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>workable-annoyance-fold-strictly-prhi</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>favourable-browsing-agreed-urgently</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>fledgling-success-prevented-actually-prhi</t>
+          <t>wellbred-reformer-banged-shakily</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>13:00</t>
+          <t>12:52</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ignited-souvenir-spelled-unabashedly</t>
+          <t>encouraged-christianity-cried-sternly-first</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>grouchy-depression-save-properly</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>faithful-pundit-entered-meaningfully-prhi</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>content-resentment-pop-hastily</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>handicapped-putting-bolted-bravely</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>encouraged-tracing-stop-fervently</t>
-        </is>
-      </c>
+          <t>portmanteau-brainstorming-analyse-stealthily-first</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>gilded-creator-bake-rigidly-first</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>13:10</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>deprived-outfield-wink-swiftly-prhi</t>
-        </is>
-      </c>
+          <t>12:59</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>authoritarian-rhinoceros-pedalled-hopelessly-first</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>subjective-resurgence-repaired-yawningly-prhi</t>
+          <t>incomplete-allegory-impress-certainly-first</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>incomplete-tuesday-blushed-kissingly</t>
+          <t>melancholy-formality-choke-fondly-first</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>just-retailer-skied-ferociously</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>graven-elephant-want-anxiously</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>realistic-elk-faced-questionably</t>
+          <t>speedy-tourist-contained-too-first</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>13:20</t>
+          <t>13:06</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>summary-inevitability-flooded-delightfully</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
+          <t>winnable-today-welcome-optimistically</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>devious-apologise-sighed-shakily-first</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>combat-collision-corrected-verbally</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>electoral-terry-employ-silently-prhi</t>
-        </is>
-      </c>
+          <t>penned-hedgehog-connect-verbally</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>paralyzed-plurality-part-helpfully</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>neurological-mayhem-rolled-worriedly-prhi</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>formulaic-metre-imagine-righteously-prhi</t>
+          <t>advised-recipe-surrounded-loosely</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>13:30</t>
+          <t>13:13</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>content-resentment-pop-hastily</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>diagonal-fluke-blinded-frantically-prhi</t>
-        </is>
-      </c>
+          <t>ignored-publisher-milked-famously</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>willful-staircase-back-sympathetically-prhi</t>
+          <t>one-year-illustrator-dressed-frantically</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>contraceptive-enclosure-released-heavily-first</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>worldly-college-rock-inwardly</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>angry-misunderstanding-calculate-softly-prhi</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>insane-armadillo-clap-deceivingly-prhi</t>
+          <t>haughty-boar-scrubbed-wildly</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>emergency-projection-stroke-loudly</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>13:40</t>
+          <t>13:20</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>paralyzed-plurality-part-helpfully</t>
+          <t>widen-differentiation-thawed-quarrelsomely</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>shadowy-tendency-answered-gratefully</t>
+          <t>degraded-dingo-cross-powerfully</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>unwrapped-immunization-pine-tomorrow</t>
+          <t>mocking-iris-imagine-regularly-first</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>formulaic-metre-imagine-righteously-prhi</t>
+          <t>sleek-squid-clean-monthly-first</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>dorky-grouping-fear-worriedly-prhi</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>thrifty-postponement-milk-seldom-prhi</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>worsted-nylon-tour-knottily-prhi</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>workable-annoyance-fold-strictly-prhi</t>
+          <t>recumbent-hello-shade-strictly</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>13:50</t>
+          <t>13:27</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>fraudulent-demon-screamed-rapidly</t>
+          <t>diagonal-zinnia-damage-partially</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>liver-laurels-asked-tediously-prhi</t>
+          <t>multidisciplinary-crocodile-dared-lightly</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>encouraged-tracing-stop-fervently</t>
+          <t>printed-grandeur-refused-seriously</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>neglected-regularity-promised-extremely-prhi</t>
+          <t>partisan-quorum-return-obediently-first</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>graven-elephant-want-anxiously</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>exacting-touchdown-picked-loudly</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>ignited-souvenir-spelled-unabashedly</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>jovial-redundancy-frightened-crazily</t>
+          <t>unparalleled-semifinal-vanish-monthly-first</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>14:00</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>clear-twenties-report-irritably-prhi</t>
-        </is>
-      </c>
+          <t>13:34</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>devilish-larceny-stretch-thoroughly-prhi</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+          <t>disgraced-counselor-use-quizzically-prhi-first</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>foolhardy-imperialism-exercised-cruelly</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>worldwide-mediator-prepared-reassuringly-prhi</t>
+          <t>interrogated-advancement-perform-certainly-prhi-first</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>aristotelian-ox-charged-hungrily</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>favourable-browsing-agreed-urgently</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>helpful-beginner-mend-exactly-prhi</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>shadowy-tendency-answered-gratefully</t>
+          <t>patriot-relaxation-press-too-prhi</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>14:10</t>
+          <t>13:41</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>diagonal-fluke-blinded-frantically-prhi</t>
+          <t>impulsive-iteration-snored-noisily-prhi</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>critical-porpoise-depend-scarily</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
+          <t>hyper-newt-alert-greedily-prhi-first</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>skeleton-function-chopped-successfully-prhi-first</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>fanciful-rationality-attempted-longingly</t>
+          <t>critical-specs-bubble-majestically-prhi</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>incalculable-validity-signed-somewhat</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>neutered-pathos-drip-fast-prhi</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>slamming-locality-mess up-quizzically-prhi</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>just-retailer-skied-ferociously</t>
+          <t>socialized-scooter-ignored-quietly-prhi</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>14:20</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>combat-collision-corrected-verbally</t>
-        </is>
-      </c>
+          <t>13:48</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>jovial-redundancy-frightened-crazily</t>
+          <t>shaken-theater-argued-frankly-prhi</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>interpreted-reptile-groan-anxiously-prhi</t>
+          <t>sincere-diploma-asked-quizzically-prhi-first</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>united-syrah-repaired-somewhat</t>
+          <t>traverse-postponement-wasted-yieldingly-prhi</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>strapping-scrimmage-explode-shakily-prhi</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>uppity-endangerment-phoned-partially</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>incomplete-tuesday-blushed-kissingly</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>burial-mahogany-flash-fully-prhi</t>
+          <t>patronizing-adoption-reigned-yearly-prhi</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>14:30</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
+          <t>13:55</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>unsuccessful-earnings-haunted-defiantly-prhi</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>angry-misunderstanding-calculate-softly-prhi</t>
+          <t>irrational-delicacy-inform-frankly</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>disconnected-brewer-escaped-upbeat</t>
+          <t>sheepish-reformer-moaned-seldom-prhi-first</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>clear-twenties-report-irritably-prhi</t>
+          <t>bellied-blossom-frighten-wonderfully-prhi-first</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>critical-porpoise-depend-scarily</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>geometric-fastball-suppose-owlishly-prhi</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>subordinate-lineage-divided-kookily-prhi</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>contraceptive-enclosure-released-heavily-first</t>
+          <t>huddled-spectacle-wander-monthly-prhi</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>14:40</t>
+          <t>14:02</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>apportioned-whale-suspended-frenetically</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
+          <t>mellow-digger-removed-judgementally-prhi</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>vain-sunflower-colour-carelessly-prhi-first</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>worldly-college-rock-inwardly</t>
+          <t>irrational-saloon-rejected-violently-prhi-first</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>wellinformed-tansy-prepared-annually</t>
+          <t>anxious-vindication-tamed-badly-prhi-first</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>neglected-regularity-promised-extremely-prhi</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>devastating-drilling-reported-successfully-prhi</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>devilish-larceny-stretch-thoroughly-prhi</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>charcoal-balls-introduced-honestly</t>
+          <t>gilded-residency-grinned-shakily-prhi</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>14:50</t>
+          <t>14:09</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>recurrent-sloth-decay-eagerly</t>
+          <t>derisive-dahlia-polished-gently-prhi-first</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>aristotelian-ox-charged-hungrily</t>
+          <t>dorky-spaghetti-hurried-questioningly-prhi-first</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>combined-saucer-destroy-sedately</t>
+          <t>detective-brotherhood-label-smoothly</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>fraudulent-demon-screamed-rapidly</t>
+          <t>congressional-mowing-landed-highly-first</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>unwrapped-immunization-pine-tomorrow</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>down-chimpanzee-drain-surprisingly-prhi</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>calm-owner-chopped-upright</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>15:00</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>strapping-scrimmage-explode-shakily-prhi</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>willful-staircase-back-sympathetically-prhi</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>young-canary-pleased-heavily-prhi</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>fledgling-success-prevented-actually-prhi</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>worldwide-mediator-prepared-reassuringly-prhi</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>uppity-endangerment-phoned-partially</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>15:10</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>thrifty-postponement-milk-seldom-prhi</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>dorky-grouping-fear-worriedly-prhi</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>neurological-mayhem-rolled-worriedly-prhi</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>recurrent-sloth-decay-eagerly</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>apportioned-whale-suspended-frenetically</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>faithful-pundit-entered-meaningfully-prhi</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+          <t>noncommercial-tavern-punctured-viciously-prhi</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>